<commit_message>
code changes as per the comments
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata/testdata.xlsx
+++ b/src/main/resources/Testdata/testdata.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830"/>
+    <workbookView windowWidth="20490" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Productdetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -33,6 +34,15 @@
   <si>
     <t>English (UK)</t>
   </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Blair's</t>
+  </si>
+  <si>
+    <t>Brazos Legends</t>
+  </si>
 </sst>
 </file>
 
@@ -62,6 +72,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -69,7 +86,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -91,7 +116,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -99,6 +124,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -107,20 +148,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -128,9 +169,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,37 +185,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,31 +216,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,31 +360,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,19 +372,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,66 +390,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -375,18 +397,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,9 +412,29 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -425,21 +455,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -454,13 +469,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,19 +507,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -518,130 +528,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -969,7 +979,7 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1009,4 +1019,39 @@
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
code updated with Assessment feedback points
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata/testdata.xlsx
+++ b/src/main/resources/Testdata/testdata.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Productdetails" sheetId="2" r:id="rId2"/>
+    <sheet name="Mechandise" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -42,6 +43,48 @@
   </si>
   <si>
     <t>Brazos Legends</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>productname</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>personlized_Name</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Hawt Like a Habanero Shirt (Men's)</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Mens</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Hawt Like a Habanero Shirt (Women's)</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -49,10 +92,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -72,6 +115,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -79,14 +129,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -94,7 +137,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -115,13 +158,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -146,31 +182,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -185,23 +206,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,187 +259,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,11 +455,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -454,32 +510,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,159 +536,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1026,7 +1069,7 @@
   <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1054,4 +1097,76 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
+  <cols>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="5" max="5" width="19.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="Hawt Like a Habanero Shirt (Women's)" tooltip="https://demo.broadleafcommerce.org/merchandise/hawt_like_a_habanero_womens"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>